<commit_message>
Documentatie en excell bijgewerkt
</commit_message>
<xml_diff>
--- a/analyse/Checklist Opdracht WPF Applicatie.xlsx
+++ b/analyse/Checklist Opdracht WPF Applicatie.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellen\OneDrive - Thomas More\2ITF WPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BandChecker\analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025067B-4CAF-48C8-ADBA-508C87780020}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9924"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist WPF" sheetId="2" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <t>Naam:</t>
   </si>
@@ -321,11 +322,20 @@
   <si>
     <t>Wat verdient extra aandacht bij het beoordelen van jouw project?</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Bandchecker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,9 +439,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -443,20 +450,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,6 +479,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>332726</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>4866675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01EFEA8-685D-448F-B6C8-A4827EEF3B09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="5200650"/>
+          <a:ext cx="5190476" cy="4800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>990165</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3504762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF054BF0-3A59-4C01-8783-D57E5F6254DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="933450"/>
+          <a:ext cx="3476190" cy="3504762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -733,95 +836,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="10.88671875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G1" s="13" t="s">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="B2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" ht="116.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="285.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>12</v>
@@ -829,13 +934,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>10</v>
@@ -844,7 +952,7 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="G9" s="6" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>11</v>
@@ -854,19 +962,19 @@
       <c r="A10" s="2"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -874,6 +982,9 @@
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -883,43 +994,43 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>20</v>
@@ -934,7 +1045,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -942,18 +1053,18 @@
         <v>21</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -961,20 +1072,20 @@
         <v>23</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>40</v>
@@ -989,9 +1100,9 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>43</v>
@@ -1006,52 +1117,52 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="100.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" ht="399.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1064,29 +1175,29 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>34</v>
@@ -1094,19 +1205,19 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>35</v>
@@ -1115,19 +1226,19 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>5</v>
@@ -1178,19 +1289,19 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>6</v>
@@ -1241,19 +1352,19 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>7</v>
@@ -1288,7 +1399,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>53</v>
@@ -1296,7 +1407,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>36</v>
@@ -1317,25 +1428,25 @@
       <c r="B41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>42</v>
@@ -1344,7 +1455,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>45</v>
@@ -1352,18 +1463,18 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1372,16 +1483,16 @@
       <c r="B48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="14" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1389,11 +1500,11 @@
       <c r="A50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="2"/>
@@ -1411,27 +1522,27 @@
       <c r="B53" s="7"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>3</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="71.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
@@ -1498,5 +1609,6 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>